<commit_message>
HUD & System changes
</commit_message>
<xml_diff>
--- a/Sheet.xlsx
+++ b/Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="137">
   <si>
     <t>Water</t>
   </si>
@@ -62,12 +62,6 @@
     <t>Characteristics</t>
   </si>
   <si>
-    <t>Bengings</t>
-  </si>
-  <si>
-    <t>Subbendings</t>
-  </si>
-  <si>
     <t>Spells</t>
   </si>
   <si>
@@ -434,16 +428,13 @@
     <t>cnt += sqrt(sqrt(cur_level * bonus_cnt)) / 100;</t>
   </si>
   <si>
-    <t>Skill points are used to increase skills power. Every new mastery level reached the hero gets 3 skill points.</t>
-  </si>
-  <si>
-    <t>To learn or upgrade a subbending, you need to spend some element points. It depends on how much elements does the subbending contain.</t>
-  </si>
-  <si>
-    <t>When the player choose the element</t>
-  </si>
-  <si>
-    <t>Every time the player finishes boss fight, he earn 1 element point and allows to choose the element point's attunement. They stores until the player will spend them on some subbending upgrade.</t>
+    <t>Elements</t>
+  </si>
+  <si>
+    <t>Bendings</t>
+  </si>
+  <si>
+    <t>Salvation</t>
   </si>
 </sst>
 </file>
@@ -451,7 +442,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -539,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -596,6 +587,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -622,16 +619,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -921,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L85"/>
+  <dimension ref="A1:L91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:E16"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -941,423 +935,419 @@
         <v>11</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="K1" s="24"/>
+      <c r="K1" s="26"/>
       <c r="L1" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>138</v>
-      </c>
+      <c r="A2" s="27"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="28">
+        <v>120</v>
+      </c>
+      <c r="D2" s="31">
         <v>100</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="31">
+      <c r="E2" s="29"/>
+      <c r="F2" s="32">
         <v>2</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="29">
+      <c r="G2" s="32"/>
+      <c r="H2" s="30">
         <v>100</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="19">
+      <c r="I2" s="30"/>
+      <c r="J2" s="21">
         <v>1249.5899999999999</v>
       </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="30" t="s">
-        <v>132</v>
+      <c r="K2" s="21"/>
+      <c r="L2" s="19" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3" s="28">
+        <v>118</v>
+      </c>
+      <c r="D3" s="31">
         <v>1</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="31">
+      <c r="E3" s="29"/>
+      <c r="F3" s="32">
         <v>5</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="29">
+      <c r="G3" s="32"/>
+      <c r="H3" s="30">
         <v>100</v>
       </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="19">
+      <c r="I3" s="30"/>
+      <c r="J3" s="21">
         <v>4.8018299999999998</v>
       </c>
-      <c r="K3" s="19"/>
-      <c r="L3" s="30" t="s">
-        <v>135</v>
+      <c r="K3" s="21"/>
+      <c r="L3" s="19" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="31">
+        <v>100</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="32">
+        <v>4</v>
+      </c>
+      <c r="G4" s="32"/>
+      <c r="H4" s="30">
+        <v>100</v>
+      </c>
+      <c r="I4" s="30"/>
+      <c r="J4" s="21">
+        <v>1842.93</v>
+      </c>
+      <c r="K4" s="21"/>
+      <c r="L4" s="19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="28">
+      <c r="C5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="31">
+        <v>1</v>
+      </c>
+      <c r="E5" s="29"/>
+      <c r="F5" s="32">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G5" s="32"/>
+      <c r="H5" s="30">
         <v>100</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="31">
-        <v>4</v>
-      </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="29">
-        <v>100</v>
-      </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="19">
-        <v>1842.93</v>
-      </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="30" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" s="28">
-        <v>1</v>
-      </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="31">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="29">
-        <v>100</v>
-      </c>
-      <c r="I5" s="29"/>
-      <c r="J5" s="19">
+      <c r="I5" s="30"/>
+      <c r="J5" s="21">
         <v>2.1618499999999998</v>
       </c>
-      <c r="K5" s="19"/>
-      <c r="L5" s="30" t="s">
-        <v>133</v>
+      <c r="K5" s="21"/>
+      <c r="L5" s="19" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="31">
         <v>1</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="31">
+      <c r="E6" s="29"/>
+      <c r="F6" s="32">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="29">
+      <c r="G6" s="32"/>
+      <c r="H6" s="30">
         <v>100</v>
       </c>
-      <c r="I6" s="29"/>
-      <c r="J6" s="19">
+      <c r="I6" s="30"/>
+      <c r="J6" s="21">
         <v>0.51363000000000003</v>
       </c>
-      <c r="K6" s="19"/>
-      <c r="L6" s="30" t="s">
-        <v>134</v>
+      <c r="K6" s="21"/>
+      <c r="L6" s="19" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D7" s="27">
+        <v>115</v>
+      </c>
+      <c r="D7" s="29">
         <v>0.1</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="31">
+      <c r="E7" s="29"/>
+      <c r="F7" s="32">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="29">
+      <c r="G7" s="32"/>
+      <c r="H7" s="30">
         <v>100</v>
       </c>
-      <c r="I7" s="29"/>
-      <c r="J7" s="19">
+      <c r="I7" s="30"/>
+      <c r="J7" s="21">
         <v>10.500400000000001</v>
       </c>
-      <c r="K7" s="19"/>
-      <c r="L7" s="30" t="s">
-        <v>133</v>
+      <c r="K7" s="21"/>
+      <c r="L7" s="19" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="28">
+        <v>110</v>
+      </c>
+      <c r="D8" s="31">
         <v>1</v>
       </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="31">
+      <c r="E8" s="29"/>
+      <c r="F8" s="32">
         <v>0.04</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="29">
+      <c r="G8" s="32"/>
+      <c r="H8" s="30">
         <v>100</v>
       </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="19">
+      <c r="I8" s="30"/>
+      <c r="J8" s="21">
         <v>3.9583400000000002</v>
       </c>
-      <c r="K8" s="19"/>
-      <c r="L8" s="30" t="s">
-        <v>133</v>
+      <c r="K8" s="21"/>
+      <c r="L8" s="19" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="29">
         <v>0.05</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="31">
+      <c r="E9" s="29"/>
+      <c r="F9" s="32">
         <v>1.2E-2</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="29">
+      <c r="G9" s="32"/>
+      <c r="H9" s="30">
         <v>100</v>
       </c>
-      <c r="I9" s="29"/>
-      <c r="J9" s="19">
+      <c r="I9" s="30"/>
+      <c r="J9" s="21">
         <v>0.31624999999999998</v>
       </c>
-      <c r="K9" s="19"/>
-      <c r="L9" s="30" t="s">
-        <v>133</v>
+      <c r="K9" s="21"/>
+      <c r="L9" s="19" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D10" s="27">
+        <v>113</v>
+      </c>
+      <c r="D10" s="29">
         <v>1.5</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="19">
+      <c r="E10" s="29"/>
+      <c r="F10" s="21">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="29">
+      <c r="G10" s="21"/>
+      <c r="H10" s="30">
         <v>100</v>
       </c>
-      <c r="I10" s="29"/>
-      <c r="J10" s="19">
+      <c r="I10" s="30"/>
+      <c r="J10" s="21">
         <v>6.1474000000000002</v>
       </c>
-      <c r="K10" s="19"/>
-      <c r="L10" s="30" t="s">
-        <v>133</v>
+      <c r="K10" s="21"/>
+      <c r="L10" s="19" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="7" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="27">
+        <v>117</v>
+      </c>
+      <c r="D11" s="29">
         <v>0.5</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="31">
+      <c r="E11" s="29"/>
+      <c r="F11" s="32">
         <v>0.1</v>
       </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="29">
+      <c r="G11" s="32"/>
+      <c r="H11" s="30">
         <v>100</v>
       </c>
-      <c r="I11" s="29"/>
-      <c r="J11" s="19">
+      <c r="I11" s="30"/>
+      <c r="J11" s="21">
         <v>18.989599999999999</v>
       </c>
-      <c r="K11" s="19"/>
-      <c r="L11" s="30" t="s">
-        <v>133</v>
+      <c r="K11" s="21"/>
+      <c r="L11" s="19" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C12" s="18"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
     </row>
     <row r="13" spans="1:12" s="12" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="I13" s="24"/>
+      <c r="I13" s="26"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>139</v>
-      </c>
+      <c r="A14" s="28"/>
       <c r="B14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
+        <v>2</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+        <v>3</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
       <c r="B17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+        <v>4</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
       <c r="B18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-    </row>
-    <row r="19" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+    </row>
+    <row r="19" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="18"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-    </row>
-    <row r="20" spans="1:9" s="12" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+    </row>
+    <row r="20" spans="1:12" s="12" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D20" s="11">
         <v>1</v>
@@ -1375,27 +1365,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
-        <v>137</v>
-      </c>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
       <c r="B21" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
       <c r="B22" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>2</v>
@@ -1403,14 +1391,15 @@
       <c r="E22" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+      <c r="J22" s="20"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
       <c r="B23" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>2</v>
@@ -1418,14 +1407,15 @@
       <c r="E23" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
+      <c r="J23" s="20"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="28"/>
       <c r="B24" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>0</v>
@@ -1436,14 +1426,15 @@
       <c r="F24" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
+      <c r="J24" s="20"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
       <c r="B25" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>2</v>
@@ -1454,14 +1445,16 @@
       <c r="F25" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
       <c r="B26" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>0</v>
@@ -1475,26 +1468,30 @@
       <c r="G26" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
       <c r="B27" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
       <c r="B28" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>0</v>
@@ -1502,14 +1499,16 @@
       <c r="E28" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
       <c r="B29" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>0</v>
@@ -1517,14 +1516,16 @@
       <c r="E29" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
       <c r="B30" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>0</v>
@@ -1535,14 +1536,16 @@
       <c r="F30" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
       <c r="B31" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>0</v>
@@ -1553,14 +1556,17 @@
       <c r="F31" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="28"/>
       <c r="B32" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>0</v>
@@ -1574,26 +1580,32 @@
       <c r="G32" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
       <c r="B33" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="28"/>
       <c r="B34" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>2</v>
@@ -1601,29 +1613,30 @@
       <c r="E34" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="J34" s="20"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="28"/>
       <c r="B35" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="28"/>
       <c r="B36" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>0</v>
@@ -1635,13 +1648,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="28"/>
       <c r="B37" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>2</v>
@@ -1653,13 +1666,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="28"/>
       <c r="B38" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>0</v>
@@ -1674,25 +1687,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="28"/>
       <c r="B39" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="28"/>
       <c r="B40" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>3</v>
@@ -1701,13 +1714,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="28"/>
       <c r="B41" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>4</v>
@@ -1716,13 +1729,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="28"/>
       <c r="B42" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>0</v>
@@ -1734,13 +1747,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="28"/>
       <c r="B43" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>3</v>
@@ -1752,13 +1765,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="28"/>
       <c r="B44" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>2</v>
@@ -1773,40 +1786,40 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="26"/>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="28"/>
       <c r="B45" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="28"/>
       <c r="B46" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="28"/>
       <c r="B47" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>0</v>
@@ -1815,13 +1828,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="28"/>
       <c r="B48" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>0</v>
@@ -1834,12 +1847,12 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="26"/>
+      <c r="A49" s="28"/>
       <c r="B49" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>2</v>
@@ -1852,12 +1865,12 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
+      <c r="A50" s="28"/>
       <c r="B50" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>0</v>
@@ -1876,12 +1889,12 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="26"/>
+      <c r="A51" s="28"/>
       <c r="B51" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>0</v>
@@ -1902,497 +1915,538 @@
     </row>
     <row r="53" spans="1:9" s="12" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="G53" s="25"/>
+      <c r="H53" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="I53" s="25"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="28"/>
+      <c r="B54" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="28"/>
+      <c r="B55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+      <c r="I55" s="21"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="28"/>
+      <c r="B56" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D56" s="22"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="28"/>
+      <c r="B57" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="28"/>
+      <c r="B58" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D58" s="22"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="28"/>
+      <c r="B59" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="28"/>
+      <c r="B60" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="28"/>
+      <c r="B61" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="28"/>
+      <c r="B62" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="21"/>
+      <c r="H62" s="21"/>
+      <c r="I62" s="21"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="28"/>
+      <c r="B63" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="28"/>
+      <c r="B64" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="28"/>
+      <c r="B65" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="21"/>
+      <c r="H65" s="21"/>
+      <c r="I65" s="21"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="28"/>
+      <c r="B66" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D66" s="22"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="21"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="28"/>
+      <c r="B67" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C53" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D53" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="G53" s="23"/>
-      <c r="H53" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="I53" s="23"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="B54" s="7" t="s">
+      <c r="C67" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="21"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="28"/>
+      <c r="B68" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="21"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="28"/>
+      <c r="B69" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="21"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="28"/>
+      <c r="B70" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="21"/>
+      <c r="H70" s="21"/>
+      <c r="I70" s="21"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="28"/>
+      <c r="B71" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="21"/>
+      <c r="H71" s="21"/>
+      <c r="I71" s="21"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="28"/>
+      <c r="B72" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C72" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="21"/>
+      <c r="H72" s="21"/>
+      <c r="I72" s="21"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="28"/>
+      <c r="B73" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="21"/>
+      <c r="H73" s="21"/>
+      <c r="I73" s="21"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="28"/>
+      <c r="B74" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="28"/>
+      <c r="B75" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D75" s="22"/>
+      <c r="E75" s="22"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="21"/>
+      <c r="H75" s="21"/>
+      <c r="I75" s="21"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="28"/>
+      <c r="B76" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D76" s="22"/>
+      <c r="E76" s="22"/>
+      <c r="F76" s="21"/>
+      <c r="G76" s="21"/>
+      <c r="H76" s="21"/>
+      <c r="I76" s="21"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="28"/>
+      <c r="B77" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D77" s="22"/>
+      <c r="E77" s="22"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="21"/>
+      <c r="H77" s="21"/>
+      <c r="I77" s="21"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="28"/>
+      <c r="B78" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D78" s="22"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="21"/>
+      <c r="H78" s="21"/>
+      <c r="I78" s="21"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="28"/>
+      <c r="B79" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="19"/>
-      <c r="I54" s="19"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
-      <c r="B55" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C55" s="2" t="s">
+      <c r="D79" s="22"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="21"/>
+      <c r="H79" s="21"/>
+      <c r="I79" s="21"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="28"/>
+      <c r="B80" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="19"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="26"/>
-      <c r="B56" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="19"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
-      <c r="B57" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="19"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="26"/>
-      <c r="B58" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
-      <c r="B59" s="7" t="s">
+      <c r="D80" s="22"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="21"/>
+      <c r="G80" s="21"/>
+      <c r="H80" s="21"/>
+      <c r="I80" s="21"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="28"/>
+      <c r="B81" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="21"/>
+      <c r="G81" s="21"/>
+      <c r="H81" s="21"/>
+      <c r="I81" s="21"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="28"/>
+      <c r="B82" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="21"/>
+      <c r="G82" s="21"/>
+      <c r="H82" s="21"/>
+      <c r="I82" s="21"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="28"/>
+      <c r="B83" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="19"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="26"/>
-      <c r="B60" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="26"/>
-      <c r="B61" s="5" t="s">
+      <c r="D83" s="22"/>
+      <c r="E83" s="22"/>
+      <c r="F83" s="21"/>
+      <c r="G83" s="21"/>
+      <c r="H83" s="21"/>
+      <c r="I83" s="21"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="28"/>
+      <c r="B84" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="19"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="19"/>
-      <c r="I61" s="19"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="26"/>
-      <c r="B62" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="19"/>
-      <c r="H62" s="19"/>
-      <c r="I62" s="19"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="26"/>
-      <c r="B63" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="26"/>
-      <c r="B64" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="19"/>
-      <c r="H64" s="19"/>
-      <c r="I64" s="19"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="26"/>
-      <c r="B65" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D65" s="20"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="19"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="26"/>
-      <c r="B66" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="19"/>
-      <c r="H66" s="19"/>
-      <c r="I66" s="19"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="26"/>
-      <c r="B67" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="19"/>
-      <c r="G67" s="19"/>
-      <c r="H67" s="19"/>
-      <c r="I67" s="19"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="26"/>
-      <c r="B68" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D68" s="20"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="19"/>
-      <c r="H68" s="19"/>
-      <c r="I68" s="19"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="26"/>
-      <c r="B69" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C69" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D69" s="20"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="19"/>
-      <c r="H69" s="19"/>
-      <c r="I69" s="19"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="26"/>
-      <c r="B70" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D70" s="20"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="19"/>
-      <c r="G70" s="19"/>
-      <c r="H70" s="19"/>
-      <c r="I70" s="19"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="26"/>
-      <c r="B71" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D71" s="20"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="19"/>
-      <c r="G71" s="19"/>
-      <c r="H71" s="19"/>
-      <c r="I71" s="19"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="26"/>
-      <c r="B72" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D72" s="20"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="19"/>
-      <c r="G72" s="19"/>
-      <c r="H72" s="19"/>
-      <c r="I72" s="19"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="26"/>
-      <c r="B73" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D73" s="20"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="19"/>
-      <c r="G73" s="19"/>
-      <c r="H73" s="19"/>
-      <c r="I73" s="19"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="26"/>
-      <c r="B74" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D74" s="20"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="19"/>
-      <c r="G74" s="19"/>
-      <c r="H74" s="19"/>
-      <c r="I74" s="19"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="26"/>
-      <c r="B75" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D75" s="20"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="19"/>
-      <c r="G75" s="19"/>
-      <c r="H75" s="19"/>
-      <c r="I75" s="19"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="26"/>
-      <c r="B76" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D76" s="20"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="19"/>
-      <c r="G76" s="19"/>
-      <c r="H76" s="19"/>
-      <c r="I76" s="19"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="26"/>
-      <c r="B77" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D77" s="20"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="19"/>
-      <c r="G77" s="19"/>
-      <c r="H77" s="19"/>
-      <c r="I77" s="19"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="26"/>
-      <c r="B78" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C78" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D78" s="20"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="19"/>
-      <c r="G78" s="19"/>
-      <c r="H78" s="19"/>
-      <c r="I78" s="19"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="26"/>
-      <c r="B79" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D79" s="20"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="19"/>
-      <c r="G79" s="19"/>
-      <c r="H79" s="19"/>
-      <c r="I79" s="19"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="26"/>
-      <c r="B80" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D80" s="20"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="19"/>
-      <c r="G80" s="19"/>
-      <c r="H80" s="19"/>
-      <c r="I80" s="19"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="26"/>
-      <c r="B81" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C81" s="10" t="s">
+      <c r="C84" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D81" s="20"/>
-      <c r="E81" s="20"/>
-      <c r="F81" s="19"/>
-      <c r="G81" s="19"/>
-      <c r="H81" s="19"/>
-      <c r="I81" s="19"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="26"/>
-      <c r="B82" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D82" s="20"/>
-      <c r="E82" s="20"/>
-      <c r="F82" s="19"/>
-      <c r="G82" s="19"/>
-      <c r="H82" s="19"/>
-      <c r="I82" s="19"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="26"/>
-      <c r="B83" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D83" s="20"/>
-      <c r="E83" s="20"/>
-      <c r="F83" s="19"/>
-      <c r="G83" s="19"/>
-      <c r="H83" s="19"/>
-      <c r="I83" s="19"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="26"/>
-      <c r="B84" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C84" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D84" s="20"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="19"/>
-      <c r="G84" s="19"/>
-      <c r="H84" s="19"/>
-      <c r="I84" s="19"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="22"/>
+      <c r="F84" s="21"/>
+      <c r="G84" s="21"/>
+      <c r="H84" s="21"/>
+      <c r="I84" s="21"/>
     </row>
     <row r="85" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C85" s="18"/>
       <c r="D85" s="18"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D86" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="20"/>
+      <c r="C87" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C88" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C89" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C90" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C91" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="166">

</xml_diff>